<commit_message>
updated to use dict instead of list for populating columns. Now mapped and also added column formatting.
</commit_message>
<xml_diff>
--- a/a_20180412_064608761.xlsx
+++ b/a_20180412_064608761.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" state="visible" r:id="rId2"/>
@@ -3882,7 +3882,7 @@
   </sheetPr>
   <dimension ref="A1:AH256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
@@ -16306,7 +16306,7 @@
   <dimension ref="A1:L256"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20455,7 +20455,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="36.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="26.13"/>
@@ -23053,14 +23053,16 @@
   </sheetPr>
   <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="53.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="44.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>